<commit_message>
Added few java files and packages are renamed
</commit_message>
<xml_diff>
--- a/pom/resources/CrmData.xlsx
+++ b/pom/resources/CrmData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>FirstName</t>
   </si>
@@ -28,19 +28,53 @@
   </si>
   <si>
     <t>PhoneNumber</t>
+  </si>
+  <si>
+    <t>Shiva</t>
+  </si>
+  <si>
+    <t>Prasad</t>
+  </si>
+  <si>
+    <t>shivav09@gmail.com</t>
+  </si>
+  <si>
+    <t>Sri</t>
+  </si>
+  <si>
+    <t>Ramya</t>
+  </si>
+  <si>
+    <t>sriramya@gm.com</t>
+  </si>
+  <si>
+    <t>Ravi</t>
+  </si>
+  <si>
+    <t>Reddy</t>
+  </si>
+  <si>
+    <t>reddyravi@gm.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -60,13 +94,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -359,13 +399,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -381,7 +427,54 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>9849522415</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3">
+        <v>8688862547</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>9878965412</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>